<commit_message>
Added legend Rooms.txt, color coded BoardLayout
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,7 +102,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,12 +118,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,17 +147,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Style 1" xfId="1"/>
+    <cellStyle name="Style 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9EA2B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9EA2B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9EA2B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -416,28 +473,28 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
@@ -446,19 +503,19 @@
       <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
@@ -467,25 +524,25 @@
       <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="P1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="W1">
@@ -493,22 +550,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
@@ -517,19 +574,19 @@
       <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N2" t="s">
@@ -538,25 +595,25 @@
       <c r="O2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="W2">
@@ -565,22 +622,22 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
@@ -589,19 +646,19 @@
       <c r="H3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N3" t="s">
@@ -610,25 +667,25 @@
       <c r="O3" t="s">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="W3">
@@ -637,22 +694,22 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
@@ -661,19 +718,19 @@
       <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N4" t="s">
@@ -682,25 +739,25 @@
       <c r="O4" t="s">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="P4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U4" t="s">
-        <v>12</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="U4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="W4">
@@ -784,22 +841,22 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H6" t="s">
@@ -832,19 +889,19 @@
       <c r="Q6" t="s">
         <v>0</v>
       </c>
-      <c r="R6" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" t="s">
-        <v>10</v>
-      </c>
-      <c r="T6" t="s">
-        <v>10</v>
-      </c>
-      <c r="U6" t="s">
-        <v>10</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="R6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W6">
@@ -856,22 +913,22 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H7" t="s">
@@ -880,10 +937,10 @@
       <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L7" t="s">
@@ -904,19 +961,19 @@
       <c r="Q7" t="s">
         <v>0</v>
       </c>
-      <c r="R7" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" t="s">
-        <v>10</v>
-      </c>
-      <c r="U7" t="s">
-        <v>10</v>
-      </c>
-      <c r="V7" t="s">
+      <c r="R7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W7">
@@ -928,22 +985,22 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H8" t="s">
@@ -952,10 +1009,10 @@
       <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L8" t="s">
@@ -976,19 +1033,19 @@
       <c r="Q8" t="s">
         <v>0</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S8" t="s">
-        <v>10</v>
-      </c>
-      <c r="T8" t="s">
-        <v>10</v>
-      </c>
-      <c r="U8" t="s">
-        <v>10</v>
-      </c>
-      <c r="V8" t="s">
+      <c r="S8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W8">
@@ -997,25 +1054,25 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H9" t="s">
@@ -1024,10 +1081,10 @@
       <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L9" t="s">
@@ -1048,19 +1105,19 @@
       <c r="Q9" t="s">
         <v>0</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T9" t="s">
-        <v>10</v>
-      </c>
-      <c r="U9" t="s">
-        <v>10</v>
-      </c>
-      <c r="V9" t="s">
+      <c r="S9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W9">
@@ -1069,25 +1126,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H10" t="s">
@@ -1096,10 +1153,10 @@
       <c r="I10" t="s">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L10" t="s">
@@ -1120,19 +1177,19 @@
       <c r="Q10" t="s">
         <v>0</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S10" t="s">
-        <v>10</v>
-      </c>
-      <c r="T10" t="s">
-        <v>10</v>
-      </c>
-      <c r="U10" t="s">
-        <v>10</v>
-      </c>
-      <c r="V10" t="s">
+      <c r="S10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W10">
@@ -1141,25 +1198,25 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H11" t="s">
@@ -1168,10 +1225,10 @@
       <c r="I11" t="s">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L11" t="s">
@@ -1192,19 +1249,19 @@
       <c r="Q11" t="s">
         <v>0</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S11" t="s">
-        <v>10</v>
-      </c>
-      <c r="T11" t="s">
-        <v>10</v>
-      </c>
-      <c r="U11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V11" t="s">
+      <c r="S11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W11">
@@ -1213,25 +1270,25 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H12" t="s">
@@ -1240,10 +1297,10 @@
       <c r="I12" t="s">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L12" t="s">
@@ -1264,19 +1321,19 @@
       <c r="Q12" t="s">
         <v>0</v>
       </c>
-      <c r="R12" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" t="s">
-        <v>10</v>
-      </c>
-      <c r="T12" t="s">
-        <v>10</v>
-      </c>
-      <c r="U12" t="s">
-        <v>10</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="R12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W12">
@@ -1285,19 +1342,19 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F13" t="s">
@@ -1312,10 +1369,10 @@
       <c r="I13" t="s">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L13" t="s">
@@ -1336,19 +1393,19 @@
       <c r="Q13" t="s">
         <v>0</v>
       </c>
-      <c r="R13" t="s">
-        <v>10</v>
-      </c>
-      <c r="S13" t="s">
-        <v>10</v>
-      </c>
-      <c r="T13" t="s">
-        <v>10</v>
-      </c>
-      <c r="U13" t="s">
-        <v>10</v>
-      </c>
-      <c r="V13" t="s">
+      <c r="R13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W13">
@@ -1384,10 +1441,10 @@
       <c r="I14" t="s">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L14" t="s">
@@ -1456,10 +1513,10 @@
       <c r="I15" t="s">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L15" t="s">
@@ -1507,19 +1564,19 @@
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="s">
@@ -1552,19 +1609,19 @@
       <c r="Q16" t="s">
         <v>0</v>
       </c>
-      <c r="R16" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" t="s">
+      <c r="R16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U16" t="s">
-        <v>21</v>
-      </c>
-      <c r="V16" t="s">
+      <c r="U16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W16">
@@ -1579,19 +1636,19 @@
       <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" t="s">
@@ -1624,19 +1681,19 @@
       <c r="Q17" t="s">
         <v>0</v>
       </c>
-      <c r="R17" t="s">
-        <v>21</v>
-      </c>
-      <c r="S17" t="s">
-        <v>21</v>
-      </c>
-      <c r="T17" t="s">
-        <v>21</v>
-      </c>
-      <c r="U17" t="s">
-        <v>21</v>
-      </c>
-      <c r="V17" t="s">
+      <c r="R17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W17">
@@ -1645,49 +1702,49 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K18" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" t="s">
-        <v>7</v>
-      </c>
-      <c r="M18" t="s">
-        <v>7</v>
-      </c>
-      <c r="N18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O18" t="s">
+      <c r="K18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="P18" t="s">
@@ -1696,19 +1753,19 @@
       <c r="Q18" t="s">
         <v>0</v>
       </c>
-      <c r="R18" t="s">
-        <v>21</v>
-      </c>
-      <c r="S18" t="s">
-        <v>21</v>
-      </c>
-      <c r="T18" t="s">
-        <v>21</v>
-      </c>
-      <c r="U18" t="s">
-        <v>21</v>
-      </c>
-      <c r="V18" t="s">
+      <c r="R18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W18">
@@ -1717,49 +1774,49 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I19" t="s">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" t="s">
-        <v>7</v>
-      </c>
-      <c r="L19" t="s">
-        <v>7</v>
-      </c>
-      <c r="M19" t="s">
-        <v>7</v>
-      </c>
-      <c r="N19" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="J19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P19" t="s">
@@ -1768,19 +1825,19 @@
       <c r="Q19" t="s">
         <v>0</v>
       </c>
-      <c r="R19" t="s">
-        <v>21</v>
-      </c>
-      <c r="S19" t="s">
-        <v>21</v>
-      </c>
-      <c r="T19" t="s">
-        <v>21</v>
-      </c>
-      <c r="U19" t="s">
-        <v>21</v>
-      </c>
-      <c r="V19" t="s">
+      <c r="R19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W19">
@@ -1789,49 +1846,49 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I20" t="s">
         <v>0</v>
       </c>
-      <c r="J20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" t="s">
-        <v>7</v>
-      </c>
-      <c r="L20" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" t="s">
-        <v>7</v>
-      </c>
-      <c r="N20" t="s">
-        <v>7</v>
-      </c>
-      <c r="O20" t="s">
+      <c r="J20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P20" t="s">
@@ -1840,19 +1897,19 @@
       <c r="Q20" t="s">
         <v>0</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S20" t="s">
-        <v>21</v>
-      </c>
-      <c r="T20" t="s">
-        <v>21</v>
-      </c>
-      <c r="U20" t="s">
-        <v>21</v>
-      </c>
-      <c r="V20" t="s">
+      <c r="S20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W20">
@@ -1861,49 +1918,49 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I21" t="s">
         <v>0</v>
       </c>
-      <c r="J21" t="s">
-        <v>7</v>
-      </c>
-      <c r="K21" t="s">
-        <v>7</v>
-      </c>
-      <c r="L21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21" t="s">
-        <v>7</v>
-      </c>
-      <c r="N21" t="s">
-        <v>7</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="J21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P21" t="s">
@@ -1912,19 +1969,19 @@
       <c r="Q21" t="s">
         <v>0</v>
       </c>
-      <c r="R21" t="s">
-        <v>21</v>
-      </c>
-      <c r="S21" t="s">
-        <v>21</v>
-      </c>
-      <c r="T21" t="s">
-        <v>21</v>
-      </c>
-      <c r="U21" t="s">
-        <v>21</v>
-      </c>
-      <c r="V21" t="s">
+      <c r="R21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W21">
@@ -1933,49 +1990,49 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I22" t="s">
         <v>0</v>
       </c>
-      <c r="J22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" t="s">
-        <v>7</v>
-      </c>
-      <c r="L22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" t="s">
-        <v>7</v>
-      </c>
-      <c r="O22" t="s">
+      <c r="J22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P22" t="s">
@@ -1984,19 +2041,19 @@
       <c r="Q22" t="s">
         <v>0</v>
       </c>
-      <c r="R22" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" t="s">
-        <v>21</v>
-      </c>
-      <c r="T22" t="s">
-        <v>21</v>
-      </c>
-      <c r="U22" t="s">
-        <v>21</v>
-      </c>
-      <c r="V22" t="s">
+      <c r="R22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W22">
@@ -2088,6 +2145,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:V22">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Spreadsheet with key
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\306\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="31">
   <si>
     <t>W</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>CL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 25</t>
+  </si>
+  <si>
+    <t>White: Door Direction Tests</t>
+  </si>
+  <si>
+    <t>Orange: Adjacency List tests inside room</t>
+  </si>
+  <si>
+    <t>Purple: Adjacency list tests room exits</t>
+  </si>
+  <si>
+    <t>Green: Adjacency lists besides room entrance</t>
+  </si>
+  <si>
+    <t>Gray Blue: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Light blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -118,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +158,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,10 +209,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,9 +243,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -470,16 +537,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A30" sqref="A1:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -497,7 +564,7 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
@@ -643,7 +710,7 @@
       <c r="G3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -667,7 +734,7 @@
       <c r="O3" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -694,7 +761,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -703,7 +770,7 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -718,7 +785,7 @@
       <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -733,7 +800,7 @@
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="O4" t="s">
@@ -787,7 +854,7 @@
       <c r="G5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -826,7 +893,7 @@
       <c r="T5" t="s">
         <v>0</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V5" t="s">
@@ -859,7 +926,7 @@
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I6" t="s">
@@ -868,7 +935,7 @@
       <c r="J6" t="s">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="L6" t="s">
@@ -937,10 +1004,10 @@
       <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="L7" t="s">
@@ -961,7 +1028,7 @@
       <c r="Q7" t="s">
         <v>0</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="S7" s="2" t="s">
@@ -1000,10 +1067,10 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I8" t="s">
@@ -1072,7 +1139,7 @@
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H9" t="s">
@@ -1111,7 +1178,7 @@
       <c r="S9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="U9" s="2" t="s">
@@ -1174,7 +1241,7 @@
       <c r="P10" t="s">
         <v>0</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>0</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1249,7 +1316,7 @@
       <c r="Q11" t="s">
         <v>0</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="S11" s="2" t="s">
@@ -1354,7 +1421,7 @@
       <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F13" t="s">
@@ -1414,7 +1481,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B14" t="s">
@@ -1426,7 +1493,7 @@
       <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="s">
@@ -1435,7 +1502,7 @@
       <c r="G14" t="s">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I14" t="s">
@@ -1459,7 +1526,7 @@
       <c r="O14" t="s">
         <v>18</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q14" t="s">
@@ -1516,7 +1583,7 @@
       <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L15" t="s">
@@ -1558,7 +1625,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
@@ -1570,7 +1637,7 @@
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1585,7 +1652,7 @@
       <c r="I16" t="s">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="9" t="s">
         <v>0</v>
       </c>
       <c r="K16" t="s">
@@ -1612,7 +1679,7 @@
       <c r="R16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="10" t="s">
         <v>22</v>
       </c>
       <c r="T16" s="1" t="s">
@@ -1735,7 +1802,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -1750,7 +1817,7 @@
       <c r="P18" t="s">
         <v>0</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -2038,7 +2105,7 @@
       <c r="P22" t="s">
         <v>0</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="R22" s="2" t="s">
@@ -2144,13 +2211,48 @@
         <v>21</v>
       </c>
     </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:V22">
+  <conditionalFormatting sqref="A2:V2 A9:V9 A8:G8 I8:V8 A17:V17 B16:I16 K16:V16 A11:V13 A10:P10 R10:V10 A7:V7 L6:V6 A5:G6 A4:M4 O4:V4 A15:V15 B14:D14 Q14:V14 A1:F1 H1:V1 I5:T5 I14:O14 A22:P22 R22:V22 V5 F14:G14 A19:V21 A18:P18 R18:V18 I6:J6 A3:G3 I3:V3 A24:A30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"W"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished failing tests for our board
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\306\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -209,7 +209,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -221,20 +221,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="1"/>
     <cellStyle name="Style 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -246,13 +241,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9EA2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -540,7 +528,7 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A1:W30"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +701,7 @@
       <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1004,7 +992,7 @@
       <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="12" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -1067,7 +1055,7 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1616,7 +1604,7 @@
       <c r="U15" t="s">
         <v>0</v>
       </c>
-      <c r="V15" t="s">
+      <c r="V15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W15">
@@ -2247,11 +2235,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:V2 A9:V9 A8:G8 I8:V8 A17:V17 B16:I16 K16:V16 A11:V13 A10:P10 R10:V10 A7:V7 L6:V6 A5:G6 A4:M4 O4:V4 A15:V15 B14:D14 Q14:V14 A1:F1 H1:V1 I5:T5 I14:O14 A22:P22 R22:V22 V5 F14:G14 A19:V21 A18:P18 R18:V18 I6:J6 A3:G3 I3:V3 A24:A30">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A2:V2 A9:V9 A8:G8 I8:V8 A17:V17 B16:I16 K16:V16 A11:V13 A10:P10 R10:V10 A7:V7 L6:V6 A5:G6 A4:M4 O4:V4 A15:U15 B14:D14 Q14:V14 A1:F1 H1:V1 I5:T5 I14:O14 A22:P22 R22:V22 V5 F14:G14 A19:V21 A18:P18 R18:V18 I6:J6 A3:G3 I3:V3 A24:A30">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Doors displaying, change layout file to include spaces for names
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\306\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="40">
   <si>
     <t>W</t>
   </si>
@@ -117,6 +117,33 @@
   </si>
   <si>
     <t>Light blue: test targets</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>CN</t>
   </si>
 </sst>
 </file>
@@ -209,7 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -221,27 +248,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="1"/>
     <cellStyle name="Style 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9EA2B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -582,7 +596,7 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,8 +676,8 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -686,8 +700,8 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
+      <c r="J2" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>19</v>
@@ -707,8 +721,8 @@
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>12</v>
+      <c r="Q2" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>12</v>
@@ -1166,8 +1180,8 @@
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
+      <c r="B9" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -1262,8 +1276,8 @@
       <c r="I10" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>15</v>
+      <c r="J10" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>15</v>
@@ -1289,8 +1303,8 @@
       <c r="R10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="2" t="s">
-        <v>10</v>
+      <c r="S10" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>10</v>
@@ -1958,8 +1972,8 @@
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
+      <c r="B20" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
@@ -1985,8 +1999,8 @@
       <c r="J20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>7</v>
+      <c r="K20" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>7</v>
@@ -2009,8 +2023,8 @@
       <c r="R20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>21</v>
+      <c r="S20" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>21</v>

</xml_diff>